<commit_message>
DRC excel file modify 0625
</commit_message>
<xml_diff>
--- a/28nm_DRC_Layer.xlsx
+++ b/28nm_DRC_Layer.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Junung\Documents\카카오톡 받은 파일\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://postechackr-my.sharepoint.com/personal/junung_postech_ac_kr/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D172E4F-C5BA-424F-896E-5EE36FD45D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{2D172E4F-C5BA-424F-896E-5EE36FD45D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90ED62E3-78BB-40D0-9BF8-B54E06EBD9B8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="464">
   <si>
     <t>65nm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1870,6 +1870,17 @@
   <si>
     <t>(M6 with width &gt; 0.700) minimum space for run length &gt; 0.700, &gt;= 0.28</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MetalxMinSpace11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GR604e2_M6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M6 minimum space to (M6 with width &gt; 1.500), for run length &gt; 1.500, &gt;= 0.5</t>
   </si>
 </sst>
 </file>
@@ -2842,10 +2853,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C4:AA205"/>
+  <dimension ref="C4:AA206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S146" sqref="S146"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4877,144 +4888,133 @@
     <row r="142" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
-      <c r="G142" s="1"/>
+      <c r="F142" t="s">
+        <v>461</v>
+      </c>
+      <c r="G142" s="1">
+        <v>500</v>
+      </c>
+      <c r="H142" t="s">
+        <v>462</v>
+      </c>
+      <c r="I142" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="143" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
-      <c r="F143" t="s">
-        <v>278</v>
-      </c>
-      <c r="G143" s="1">
-        <v>60</v>
-      </c>
-      <c r="H143" s="2" t="s">
-        <v>297</v>
-      </c>
+      <c r="G143" s="1"/>
     </row>
     <row r="144" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
+      <c r="F144" t="s">
+        <v>278</v>
+      </c>
+      <c r="G144" s="1">
+        <v>60</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="145" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
-      <c r="F145" t="s">
-        <v>146</v>
-      </c>
-      <c r="G145" s="1">
-        <v>0</v>
-      </c>
-      <c r="H145" t="s">
-        <v>298</v>
-      </c>
-      <c r="I145" t="s">
-        <v>299</v>
-      </c>
     </row>
     <row r="146" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
       <c r="F146" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G146" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H146" t="s">
-        <v>219</v>
+        <v>298</v>
       </c>
       <c r="I146" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="147" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
-      <c r="E147" s="1"/>
       <c r="F147" t="s">
-        <v>279</v>
+        <v>145</v>
       </c>
       <c r="G147" s="1">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H147" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="I147" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
     </row>
     <row r="148" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
-      <c r="G148" s="1"/>
+      <c r="F148" t="s">
+        <v>279</v>
+      </c>
+      <c r="G148" s="1">
+        <v>11</v>
+      </c>
+      <c r="H148" t="s">
+        <v>282</v>
+      </c>
+      <c r="I148" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="149" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C149" s="1"/>
-      <c r="D149" s="1">
-        <v>180</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F149" t="s">
-        <v>301</v>
-      </c>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1"/>
+      <c r="G149" s="1"/>
     </row>
     <row r="150" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C150" s="1"/>
-      <c r="D150" s="1"/>
-      <c r="E150" s="1"/>
-      <c r="G150" s="1"/>
-      <c r="I150" s="3"/>
+      <c r="D150" s="1">
+        <v>180</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F150" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="151" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="D151" s="1">
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="I151" s="3"/>
+    </row>
+    <row r="152" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="D152" s="1">
         <v>188</v>
       </c>
-      <c r="E151" s="1" t="s">
+      <c r="E152" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="F151" t="s">
+      <c r="F152" t="s">
         <v>304</v>
       </c>
-      <c r="G151" s="1">
+      <c r="G152" s="1">
         <v>400</v>
       </c>
-      <c r="H151" t="s">
+      <c r="H152" t="s">
         <v>312</v>
       </c>
-      <c r="I151" s="3" t="s">
+      <c r="I152" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="J151" s="3"/>
-      <c r="K151" s="3"/>
-      <c r="L151" s="3"/>
-      <c r="M151" s="3"/>
-      <c r="N151" s="3"/>
-      <c r="O151" s="3"/>
-      <c r="P151" s="3"/>
-      <c r="Q151" s="3"/>
-    </row>
-    <row r="152" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C152" s="1"/>
-      <c r="D152" s="1"/>
-      <c r="E152" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F152" t="s">
-        <v>305</v>
-      </c>
-      <c r="G152" s="1">
-        <v>12000</v>
-      </c>
-      <c r="H152" t="s">
-        <v>318</v>
-      </c>
-      <c r="I152" s="3" t="s">
-        <v>319</v>
       </c>
       <c r="J152" s="3"/>
       <c r="K152" s="3"/>
@@ -5028,17 +5028,20 @@
     <row r="153" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
+      <c r="E153" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="F153" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G153" s="1">
-        <v>400</v>
+        <v>12000</v>
       </c>
       <c r="H153" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="I153" s="3" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="J153" s="3"/>
       <c r="K153" s="3"/>
@@ -5052,12 +5055,17 @@
     <row r="154" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
-      <c r="G154" s="1"/>
+      <c r="F154" t="s">
+        <v>306</v>
+      </c>
+      <c r="G154" s="1">
+        <v>400</v>
+      </c>
       <c r="H154" t="s">
-        <v>241</v>
+        <v>316</v>
       </c>
       <c r="I154" s="3" t="s">
-        <v>434</v>
+        <v>317</v>
       </c>
       <c r="J154" s="3"/>
       <c r="K154" s="3"/>
@@ -5071,11 +5079,12 @@
     <row r="155" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
+      <c r="G155" s="1"/>
       <c r="H155" t="s">
         <v>241</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="J155" s="3"/>
       <c r="K155" s="3"/>
@@ -5089,18 +5098,13 @@
     <row r="156" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
-      <c r="F156" t="s">
-        <v>307</v>
-      </c>
-      <c r="G156" s="1">
-        <v>800</v>
-      </c>
       <c r="H156" t="s">
-        <v>439</v>
+        <v>241</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>440</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="J156" s="3"/>
       <c r="K156" s="3"/>
       <c r="L156" s="3"/>
       <c r="M156" s="3"/>
@@ -5112,14 +5116,18 @@
     <row r="157" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
-      <c r="G157" s="1"/>
+      <c r="F157" t="s">
+        <v>307</v>
+      </c>
+      <c r="G157" s="1">
+        <v>800</v>
+      </c>
       <c r="H157" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="J157" s="3"/>
+        <v>440</v>
+      </c>
       <c r="K157" s="3"/>
       <c r="L157" s="3"/>
       <c r="M157" s="3"/>
@@ -5131,17 +5139,12 @@
     <row r="158" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
-      <c r="F158" t="s">
-        <v>308</v>
-      </c>
-      <c r="G158" s="1">
-        <v>1600</v>
-      </c>
+      <c r="G158" s="1"/>
       <c r="H158" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="J158" s="3"/>
       <c r="K158" s="3"/>
@@ -5155,8 +5158,18 @@
     <row r="159" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
-      <c r="G159" s="1"/>
-      <c r="I159" s="3"/>
+      <c r="F159" t="s">
+        <v>308</v>
+      </c>
+      <c r="G159" s="1">
+        <v>1600</v>
+      </c>
+      <c r="H159" t="s">
+        <v>436</v>
+      </c>
+      <c r="I159" s="3" t="s">
+        <v>435</v>
+      </c>
       <c r="J159" s="3"/>
       <c r="K159" s="3"/>
       <c r="L159" s="3"/>
@@ -5169,18 +5182,8 @@
     <row r="160" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
-      <c r="F160" t="s">
-        <v>309</v>
-      </c>
-      <c r="G160" s="1">
-        <v>20</v>
-      </c>
-      <c r="H160" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="I160" t="s">
-        <v>244</v>
-      </c>
+      <c r="G160" s="1"/>
+      <c r="I160" s="3"/>
       <c r="J160" s="3"/>
       <c r="K160" s="3"/>
       <c r="L160" s="3"/>
@@ -5194,16 +5197,16 @@
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
       <c r="F161" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G161" s="1">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="I161" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="J161" s="3"/>
       <c r="K161" s="3"/>
@@ -5218,16 +5221,16 @@
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
       <c r="F162" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G162" s="1">
-        <v>480</v>
-      </c>
-      <c r="H162" t="s">
-        <v>313</v>
-      </c>
-      <c r="I162" s="3" t="s">
-        <v>315</v>
+        <v>80</v>
+      </c>
+      <c r="H162" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I162" t="s">
+        <v>258</v>
       </c>
       <c r="J162" s="3"/>
       <c r="K162" s="3"/>
@@ -5241,9 +5244,18 @@
     <row r="163" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
-      <c r="E163" s="1"/>
-      <c r="G163" s="1"/>
-      <c r="I163" s="3"/>
+      <c r="F163" t="s">
+        <v>311</v>
+      </c>
+      <c r="G163" s="1">
+        <v>480</v>
+      </c>
+      <c r="H163" t="s">
+        <v>313</v>
+      </c>
+      <c r="I163" s="3" t="s">
+        <v>315</v>
+      </c>
       <c r="J163" s="3"/>
       <c r="K163" s="3"/>
       <c r="L163" s="3"/>
@@ -5270,24 +5282,10 @@
     </row>
     <row r="165" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C165" s="1"/>
-      <c r="D165" s="1">
-        <v>194</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F165" t="s">
-        <v>321</v>
-      </c>
-      <c r="G165" s="1">
-        <v>4000</v>
-      </c>
-      <c r="H165" t="s">
-        <v>329</v>
-      </c>
-      <c r="I165" s="3" t="s">
-        <v>330</v>
-      </c>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1"/>
+      <c r="G165" s="1"/>
+      <c r="I165" s="3"/>
       <c r="J165" s="3"/>
       <c r="K165" s="3"/>
       <c r="L165" s="3"/>
@@ -5299,15 +5297,24 @@
     </row>
     <row r="166" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C166" s="1"/>
-      <c r="D166" s="1"/>
-      <c r="E166" s="1"/>
+      <c r="D166" s="1">
+        <v>194</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="F166" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G166" s="1">
-        <v>12000</v>
-      </c>
-      <c r="I166" s="3"/>
+        <v>4000</v>
+      </c>
+      <c r="H166" t="s">
+        <v>329</v>
+      </c>
+      <c r="I166" s="3" t="s">
+        <v>330</v>
+      </c>
       <c r="J166" s="3"/>
       <c r="K166" s="3"/>
       <c r="L166" s="3"/>
@@ -5322,17 +5329,12 @@
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
       <c r="F167" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G167" s="1">
-        <v>2000</v>
-      </c>
-      <c r="H167" t="s">
-        <v>331</v>
-      </c>
-      <c r="I167" s="3" t="s">
-        <v>332</v>
-      </c>
+        <v>12000</v>
+      </c>
+      <c r="I167" s="3"/>
       <c r="J167" s="3"/>
       <c r="K167" s="3"/>
       <c r="L167" s="3"/>
@@ -5347,15 +5349,17 @@
       <c r="D168" s="1"/>
       <c r="E168" s="1"/>
       <c r="F168" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G168" s="1">
         <v>2000</v>
       </c>
       <c r="H168" t="s">
-        <v>241</v>
-      </c>
-      <c r="I168" s="3"/>
+        <v>331</v>
+      </c>
+      <c r="I168" s="3" t="s">
+        <v>332</v>
+      </c>
       <c r="J168" s="3"/>
       <c r="K168" s="3"/>
       <c r="L168" s="3"/>
@@ -5370,7 +5374,7 @@
       <c r="D169" s="1"/>
       <c r="E169" s="1"/>
       <c r="F169" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G169" s="1">
         <v>2000</v>
@@ -5392,7 +5396,15 @@
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
-      <c r="G170" s="1"/>
+      <c r="F170" t="s">
+        <v>325</v>
+      </c>
+      <c r="G170" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H170" t="s">
+        <v>241</v>
+      </c>
       <c r="I170" s="3"/>
       <c r="J170" s="3"/>
       <c r="K170" s="3"/>
@@ -5407,18 +5419,8 @@
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
-      <c r="F171" t="s">
-        <v>326</v>
-      </c>
-      <c r="G171" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H171" t="s">
-        <v>263</v>
-      </c>
-      <c r="I171" s="3" t="s">
-        <v>264</v>
-      </c>
+      <c r="G171" s="1"/>
+      <c r="I171" s="3"/>
       <c r="J171" s="3"/>
       <c r="K171" s="3"/>
       <c r="L171" s="3"/>
@@ -5433,12 +5435,17 @@
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
       <c r="F172" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G172" s="1">
         <v>1000</v>
       </c>
-      <c r="I172" s="3"/>
+      <c r="H172" t="s">
+        <v>263</v>
+      </c>
+      <c r="I172" s="3" t="s">
+        <v>264</v>
+      </c>
       <c r="J172" s="3"/>
       <c r="K172" s="3"/>
       <c r="L172" s="3"/>
@@ -5452,7 +5459,12 @@
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
-      <c r="G173" s="1"/>
+      <c r="F173" t="s">
+        <v>327</v>
+      </c>
+      <c r="G173" s="1">
+        <v>1000</v>
+      </c>
       <c r="I173" s="3"/>
       <c r="J173" s="3"/>
       <c r="K173" s="3"/>
@@ -5467,15 +5479,7 @@
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
-      <c r="F174" t="s">
-        <v>328</v>
-      </c>
-      <c r="G174" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="H174" t="s">
-        <v>241</v>
-      </c>
+      <c r="G174" s="1"/>
       <c r="I174" s="3"/>
       <c r="J174" s="3"/>
       <c r="K174" s="3"/>
@@ -5490,7 +5494,15 @@
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
-      <c r="G175" s="1"/>
+      <c r="F175" t="s">
+        <v>328</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H175" t="s">
+        <v>241</v>
+      </c>
       <c r="I175" s="3"/>
       <c r="J175" s="3"/>
       <c r="K175" s="3"/>
@@ -5504,37 +5516,35 @@
     <row r="176" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
-      <c r="E176" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F176" t="s">
-        <v>334</v>
-      </c>
-      <c r="G176" s="1">
-        <v>170</v>
-      </c>
-      <c r="H176" t="s">
-        <v>335</v>
-      </c>
-      <c r="I176" t="s">
-        <v>336</v>
-      </c>
+      <c r="E176" s="1"/>
+      <c r="G176" s="1"/>
+      <c r="I176" s="3"/>
+      <c r="J176" s="3"/>
+      <c r="K176" s="3"/>
+      <c r="L176" s="3"/>
+      <c r="M176" s="3"/>
+      <c r="N176" s="3"/>
+      <c r="O176" s="3"/>
+      <c r="P176" s="3"/>
+      <c r="Q176" s="3"/>
     </row>
     <row r="177" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
-      <c r="E177" s="1"/>
+      <c r="E177" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="F177" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="G177" s="1">
         <v>170</v>
       </c>
       <c r="H177" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="I177" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="178" spans="3:9" x14ac:dyDescent="0.3">
@@ -5542,16 +5552,16 @@
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
       <c r="F178" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="G178" s="1">
-        <v>95</v>
+        <v>170</v>
       </c>
       <c r="H178" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="I178" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="179" spans="3:9" x14ac:dyDescent="0.3">
@@ -5559,48 +5569,61 @@
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
       <c r="F179" t="s">
+        <v>337</v>
+      </c>
+      <c r="G179" s="1">
+        <v>95</v>
+      </c>
+      <c r="H179" t="s">
+        <v>338</v>
+      </c>
+      <c r="I179" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="180" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1"/>
+      <c r="F180" t="s">
         <v>456</v>
       </c>
-      <c r="G179" s="1">
+      <c r="G180" s="1">
         <v>160000</v>
       </c>
-      <c r="H179" t="s">
+      <c r="H180" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="180" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C180" s="9"/>
-      <c r="D180" s="1"/>
-      <c r="E180" s="1" t="s">
+    <row r="181" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C181" s="9"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="F180" t="s">
+      <c r="F181" t="s">
         <v>386</v>
       </c>
-      <c r="H180" t="s">
+      <c r="H181" t="s">
         <v>387</v>
       </c>
-      <c r="I180" t="s">
+      <c r="I181" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="181" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C181" s="1"/>
-      <c r="D181" s="1"/>
     </row>
     <row r="182" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
-      <c r="H182" t="s">
-        <v>343</v>
-      </c>
-      <c r="I182" t="s">
-        <v>344</v>
-      </c>
     </row>
     <row r="183" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
+      <c r="H183" t="s">
+        <v>343</v>
+      </c>
+      <c r="I183" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="184" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C184" s="1"/>
@@ -5643,6 +5666,7 @@
       <c r="D193" s="1"/>
     </row>
     <row r="194" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C194" s="1"/>
       <c r="D194" s="1"/>
     </row>
     <row r="195" spans="3:4" x14ac:dyDescent="0.3">
@@ -5677,6 +5701,9 @@
     </row>
     <row r="205" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D205" s="1"/>
+    </row>
+    <row r="206" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D206" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
0630 DRC & ResistorBank modify junung
</commit_message>
<xml_diff>
--- a/28nm_DRC_Layer.xlsx
+++ b/28nm_DRC_Layer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://postechackr-my.sharepoint.com/personal/junung_postech_ac_kr/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://postechackr-my.sharepoint.com/personal/junung_postech_ac_kr/Documents/연구/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{2D172E4F-C5BA-424F-896E-5EE36FD45D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90ED62E3-78BB-40D0-9BF8-B54E06EBD9B8}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{2D172E4F-C5BA-424F-896E-5EE36FD45D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{462F7C80-D1C2-4A56-97E7-2BD13CA8C48F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1530" windowWidth="24300" windowHeight="12765" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="467">
   <si>
     <t>65nm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1881,6 +1881,17 @@
   </si>
   <si>
     <t>M6 minimum space to (M6 with width &gt; 1.500), for run length &gt; 1.500, &gt;= 0.5</t>
+  </si>
+  <si>
+    <t>PpMinArea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GRB_PH04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PH (as generated by Boolean) minimum enclosed area (um2) &gt;= 0.16</t>
   </si>
 </sst>
 </file>
@@ -1939,7 +1950,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1955,6 +1966,18 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1993,7 +2016,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2025,6 +2048,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2853,10 +2882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C4:AA206"/>
+  <dimension ref="C4:AA207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F141" sqref="F141"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3002,49 +3031,50 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="S13" s="1" t="s">
+      <c r="F13" t="s">
+        <v>464</v>
+      </c>
+      <c r="G13" s="12">
+        <v>160000</v>
+      </c>
+      <c r="H13" t="s">
+        <v>465</v>
+      </c>
+      <c r="I13" t="s">
+        <v>466</v>
+      </c>
+      <c r="S13" s="8"/>
+    </row>
+    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="S14" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C14" s="1" t="s">
+    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <v>107</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G15" s="1">
         <v>140</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I15" t="s">
         <v>393</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="S15" s="4" t="s">
         <v>359</v>
-      </c>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G15" s="1">
-        <v>70</v>
-      </c>
-      <c r="I15" t="s">
-        <v>394</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.3">
@@ -3052,32 +3082,34 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>395</v>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="H16" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="G16" s="1">
+        <v>70</v>
       </c>
       <c r="I16" t="s">
-        <v>101</v>
-      </c>
-      <c r="S16" s="4" t="s">
-        <v>361</v>
+        <v>394</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
+      <c r="F17" t="s">
+        <v>395</v>
+      </c>
       <c r="G17" s="10"/>
       <c r="H17" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I17" t="s">
-        <v>97</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>242</v>
+        <v>101</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="3:27" x14ac:dyDescent="0.3">
@@ -3086,13 +3118,13 @@
       <c r="E18" s="1"/>
       <c r="G18" s="10"/>
       <c r="H18" t="s">
-        <v>351</v>
+        <v>96</v>
       </c>
       <c r="I18" t="s">
-        <v>352</v>
-      </c>
-      <c r="S18" s="4" t="s">
-        <v>362</v>
+        <v>97</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="3:27" x14ac:dyDescent="0.3">
@@ -3104,10 +3136,10 @@
         <v>351</v>
       </c>
       <c r="I19" t="s">
-        <v>353</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>363</v>
+        <v>352</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="3:27" x14ac:dyDescent="0.3">
@@ -3116,13 +3148,13 @@
       <c r="E20" s="1"/>
       <c r="G20" s="10"/>
       <c r="H20" t="s">
-        <v>389</v>
+        <v>351</v>
       </c>
       <c r="I20" t="s">
-        <v>390</v>
-      </c>
-      <c r="S20" s="4" t="s">
-        <v>364</v>
+        <v>353</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="21" spans="3:27" x14ac:dyDescent="0.3">
@@ -3131,120 +3163,114 @@
       <c r="E21" s="1"/>
       <c r="G21" s="10"/>
       <c r="H21" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I21" t="s">
-        <v>392</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>365</v>
+        <v>390</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="22" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="S22" s="4" t="s">
+      <c r="G22" s="10"/>
+      <c r="H22" t="s">
+        <v>391</v>
+      </c>
+      <c r="I22" t="s">
+        <v>392</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="S23" s="4" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="23" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C23" s="1" t="s">
+    <row r="24" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C24" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D24" s="1">
         <v>123</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G24" s="1">
         <v>30</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" t="s">
         <v>107</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" t="s">
         <v>108</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="S24" s="1" t="s">
         <v>367</v>
-      </c>
-    </row>
-    <row r="24" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="F24" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24" s="1">
-        <v>96</v>
-      </c>
-      <c r="H24" t="s">
-        <v>109</v>
-      </c>
-      <c r="I24" t="s">
-        <v>110</v>
-      </c>
-      <c r="S24" s="4" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="25" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="F25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G25" s="1">
         <v>96</v>
       </c>
-      <c r="S25" s="1" t="s">
-        <v>369</v>
+      <c r="H25" t="s">
+        <v>109</v>
+      </c>
+      <c r="I25" t="s">
+        <v>110</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="26" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="F26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G26" s="1">
-        <v>28</v>
-      </c>
-      <c r="H26" t="s">
-        <v>111</v>
-      </c>
-      <c r="I26" t="s">
-        <v>112</v>
-      </c>
-      <c r="S26" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="27" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="F27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G27" s="1">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I27" t="s">
-        <v>114</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>221</v>
+        <v>112</v>
+      </c>
+      <c r="S27" s="4" t="s">
+        <v>370</v>
       </c>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
@@ -3253,31 +3279,38 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="F28" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="G28" s="1">
-        <v>96</v>
+        <v>37</v>
+      </c>
+      <c r="H28" t="s">
+        <v>113</v>
       </c>
       <c r="I28" t="s">
-        <v>110</v>
-      </c>
-      <c r="S28" s="4" t="s">
-        <v>371</v>
+        <v>114</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
-      <c r="Y28" s="1"/>
     </row>
     <row r="29" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="F29" t="s">
-        <v>401</v>
+        <v>115</v>
       </c>
       <c r="G29" s="1">
         <v>96</v>
       </c>
-      <c r="S29" s="8"/>
+      <c r="I29" t="s">
+        <v>110</v>
+      </c>
+      <c r="S29" s="4" t="s">
+        <v>371</v>
+      </c>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="Y29" s="1"/>
@@ -3286,7 +3319,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="F30" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G30" s="1">
         <v>96</v>
@@ -3299,366 +3332,369 @@
     <row r="31" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" t="s">
-        <v>346</v>
-      </c>
-      <c r="I31" t="s">
-        <v>347</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>220</v>
-      </c>
+      <c r="F31" t="s">
+        <v>402</v>
+      </c>
+      <c r="G31" s="1">
+        <v>96</v>
+      </c>
+      <c r="S31" s="8"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="Y31" s="1"/>
-      <c r="AA31" s="1"/>
     </row>
     <row r="32" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="S32" s="4" t="s">
+      <c r="H32" t="s">
+        <v>346</v>
+      </c>
+      <c r="I32" t="s">
+        <v>347</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="AA32" s="1"/>
+    </row>
+    <row r="33" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="S33" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="U32" s="4" t="s">
+      <c r="U33" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="W32" s="4" t="s">
+      <c r="W33" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="Y32" s="4" t="s">
+      <c r="Y33" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="AA32" s="4" t="s">
+      <c r="AA33" s="4" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="33" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C33" s="1" t="s">
+    <row r="34" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D34" s="1">
         <v>158</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F34" t="s">
         <v>116</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G34" s="1">
         <v>40</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I34" t="s">
         <v>125</v>
       </c>
-      <c r="S33" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="U33" s="1" t="s">
+      <c r="U34" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="W33" s="1" t="s">
+      <c r="W34" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="Y33" s="1" t="s">
+      <c r="Y34" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="AA33" s="1" t="s">
+      <c r="AA34" s="1" t="s">
         <v>373</v>
-      </c>
-    </row>
-    <row r="34" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="F34" t="s">
-        <v>117</v>
-      </c>
-      <c r="G34" s="1">
-        <v>60</v>
-      </c>
-      <c r="H34" t="s">
-        <v>126</v>
-      </c>
-      <c r="I34" t="s">
-        <v>127</v>
-      </c>
-      <c r="N34" t="s">
-        <v>240</v>
-      </c>
-      <c r="S34" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="U34" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="W34" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="Y34" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="AA34" s="4" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="35" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="F35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G35" s="1">
         <v>60</v>
       </c>
-      <c r="S35" s="1"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="1"/>
-      <c r="Y35" s="1"/>
+      <c r="H35" t="s">
+        <v>126</v>
+      </c>
+      <c r="I35" t="s">
+        <v>127</v>
+      </c>
+      <c r="N35" t="s">
+        <v>240</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="U35" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="W35" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="Y35" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="AA35" s="4" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="36" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="F36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G36" s="1">
-        <v>92</v>
-      </c>
-      <c r="H36" t="s">
-        <v>128</v>
-      </c>
-      <c r="I36" t="s">
-        <v>129</v>
-      </c>
-      <c r="S36" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="U36" s="6" t="s">
-        <v>378</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="S36" s="1"/>
+      <c r="U36" s="5"/>
       <c r="V36" s="1"/>
-      <c r="W36" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y36" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="AA36" s="6" t="s">
-        <v>381</v>
-      </c>
+      <c r="Y36" s="1"/>
     </row>
     <row r="37" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="F37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G37" s="1">
         <v>92</v>
       </c>
-      <c r="U37" s="5"/>
+      <c r="H37" t="s">
+        <v>128</v>
+      </c>
+      <c r="I37" t="s">
+        <v>129</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="U37" s="6" t="s">
+        <v>378</v>
+      </c>
       <c r="V37" s="1"/>
-      <c r="Y37" s="1"/>
+      <c r="W37" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="Y37" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="AA37" s="6" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="38" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="F38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G38" s="1">
-        <v>14</v>
-      </c>
-      <c r="H38" t="s">
-        <v>130</v>
-      </c>
-      <c r="I38" t="s">
-        <v>131</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="U38" s="5"/>
+      <c r="V38" s="1"/>
       <c r="Y38" s="1"/>
     </row>
     <row r="39" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="F39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G39" s="1">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H39" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I39" t="s">
-        <v>133</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="Y39" s="1"/>
     </row>
     <row r="40" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="G40" s="10"/>
+      <c r="F40" t="s">
+        <v>122</v>
+      </c>
+      <c r="G40" s="1">
+        <v>20</v>
+      </c>
       <c r="H40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="F41" t="s">
-        <v>123</v>
-      </c>
-      <c r="G41" s="1">
-        <v>30</v>
-      </c>
+      <c r="G41" s="10"/>
       <c r="H41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I41" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="F42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G42" s="1">
         <v>30</v>
+      </c>
+      <c r="H42" t="s">
+        <v>136</v>
+      </c>
+      <c r="I42" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="G43" s="10"/>
-      <c r="H43" t="s">
-        <v>383</v>
-      </c>
-      <c r="I43" t="s">
-        <v>384</v>
+      <c r="F43" t="s">
+        <v>124</v>
+      </c>
+      <c r="G43" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="G44" s="10"/>
+      <c r="H44" t="s">
+        <v>383</v>
+      </c>
+      <c r="I44" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="45" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="C46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D46" s="1">
         <v>162</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F46" t="s">
         <v>138</v>
-      </c>
-      <c r="G45" s="1">
-        <v>50</v>
-      </c>
-      <c r="H45" t="s">
-        <v>150</v>
-      </c>
-      <c r="I45" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="46" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="F46" t="s">
-        <v>139</v>
       </c>
       <c r="G46" s="1">
         <v>50</v>
       </c>
       <c r="H46" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I46" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="G47" s="1"/>
+      <c r="F47" t="s">
+        <v>139</v>
+      </c>
+      <c r="G47" s="1">
+        <v>50</v>
+      </c>
+      <c r="H47" t="s">
+        <v>154</v>
+      </c>
+      <c r="I47" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="48" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="F48" t="s">
-        <v>140</v>
-      </c>
-      <c r="G48" s="1">
-        <v>65</v>
-      </c>
-      <c r="H48" t="s">
-        <v>167</v>
-      </c>
-      <c r="I48" t="s">
-        <v>414</v>
-      </c>
+      <c r="G48" s="1"/>
     </row>
     <row r="49" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="F49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G49" s="1">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="H49" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="I49" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="50" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="F50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G50" s="1">
-        <v>74</v>
+        <v>82</v>
+      </c>
+      <c r="H50" t="s">
+        <v>156</v>
+      </c>
+      <c r="I50" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="51" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="F51" t="s">
-        <v>143</v>
+      <c r="F51" s="11" t="s">
+        <v>142</v>
       </c>
       <c r="G51" s="1">
-        <v>140</v>
-      </c>
-      <c r="H51" t="s">
-        <v>288</v>
-      </c>
-      <c r="I51" t="s">
-        <v>412</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="F52" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G52" s="1">
+        <v>140</v>
+      </c>
       <c r="H52" t="s">
-        <v>165</v>
+        <v>288</v>
       </c>
       <c r="I52" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="53" spans="3:16" x14ac:dyDescent="0.3">
@@ -3666,37 +3702,37 @@
       <c r="D53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="I53" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="54" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="G54" s="1"/>
+      <c r="H54" t="s">
+        <v>157</v>
+      </c>
+      <c r="I54" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="55" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" t="s">
-        <v>158</v>
-      </c>
-      <c r="I55" t="s">
-        <v>409</v>
-      </c>
     </row>
     <row r="56" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I56" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="57" spans="3:16" x14ac:dyDescent="0.3">
@@ -3704,10 +3740,10 @@
       <c r="D57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="I57" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="58" spans="3:16" x14ac:dyDescent="0.3">
@@ -3715,128 +3751,128 @@
       <c r="D58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I58" t="s">
-        <v>405</v>
-      </c>
-      <c r="P58" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="59" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="G59" s="1"/>
+      <c r="H59" t="s">
+        <v>159</v>
+      </c>
+      <c r="I59" t="s">
+        <v>405</v>
+      </c>
+      <c r="P59" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="60" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="G60" s="1"/>
-      <c r="H60" t="s">
-        <v>415</v>
-      </c>
-      <c r="I60" t="s">
-        <v>416</v>
-      </c>
     </row>
     <row r="61" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I61" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="62" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="G62" s="1"/>
+      <c r="H62" t="s">
+        <v>417</v>
+      </c>
+      <c r="I62" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="63" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="G63" s="1"/>
-      <c r="H63" t="s">
-        <v>419</v>
-      </c>
-      <c r="I63" t="s">
-        <v>420</v>
-      </c>
     </row>
     <row r="64" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I64" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="G65" s="1"/>
+      <c r="H65" t="s">
+        <v>421</v>
+      </c>
+      <c r="I65" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="66" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="F66" t="s">
-        <v>144</v>
-      </c>
-      <c r="G66" s="1">
-        <v>60</v>
-      </c>
-      <c r="H66" t="s">
-        <v>168</v>
-      </c>
-      <c r="I66" t="s">
-        <v>169</v>
-      </c>
+      <c r="G66" s="1"/>
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="F67" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G67" s="1">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="H67" t="s">
+        <v>168</v>
       </c>
       <c r="I67" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="F68" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G68" s="1">
-        <v>17</v>
-      </c>
-      <c r="H68" t="s">
-        <v>171</v>
+        <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="G69" s="1"/>
+      <c r="F69" t="s">
+        <v>145</v>
+      </c>
+      <c r="G69" s="1">
+        <v>17</v>
+      </c>
       <c r="H69" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I69" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.3">
@@ -3844,228 +3880,228 @@
       <c r="D70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I70" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="G71" s="1"/>
+      <c r="H71" t="s">
+        <v>174</v>
+      </c>
+      <c r="I71" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
-      <c r="F72" t="s">
-        <v>147</v>
-      </c>
-      <c r="G72" s="1">
-        <v>0</v>
-      </c>
-      <c r="I72">
-        <f>0</f>
-        <v>0</v>
-      </c>
+      <c r="G72" s="1"/>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="F73" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G73" s="1">
-        <v>21</v>
-      </c>
-      <c r="H73" t="s">
-        <v>177</v>
-      </c>
-      <c r="I73" t="s">
-        <v>178</v>
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <f>0</f>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
-      <c r="G74" s="1"/>
+      <c r="F74" t="s">
+        <v>148</v>
+      </c>
+      <c r="G74" s="1">
+        <v>21</v>
+      </c>
+      <c r="H74" t="s">
+        <v>177</v>
+      </c>
+      <c r="I74" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="75" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
-      <c r="F75" t="s">
-        <v>149</v>
-      </c>
-      <c r="G75" s="1">
-        <v>10</v>
-      </c>
-      <c r="H75" t="s">
-        <v>152</v>
-      </c>
-      <c r="I75" t="s">
-        <v>153</v>
-      </c>
+      <c r="G75" s="1"/>
     </row>
     <row r="76" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
-      <c r="G76" s="1"/>
+      <c r="F76" t="s">
+        <v>149</v>
+      </c>
+      <c r="G76" s="1">
+        <v>10</v>
+      </c>
+      <c r="H76" t="s">
+        <v>152</v>
+      </c>
+      <c r="I76" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="77" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C78" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D78" s="1">
         <v>110</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E78" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F78" t="s">
         <v>180</v>
-      </c>
-      <c r="G77" s="1">
-        <v>260</v>
-      </c>
-      <c r="H77" t="s">
-        <v>349</v>
-      </c>
-      <c r="I77" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="F78" t="s">
-        <v>181</v>
       </c>
       <c r="G78" s="1">
         <v>260</v>
       </c>
       <c r="H78" t="s">
-        <v>185</v>
+        <v>349</v>
       </c>
       <c r="I78" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="79" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
-      <c r="G79" s="10"/>
+      <c r="F79" t="s">
+        <v>181</v>
+      </c>
+      <c r="G79" s="1">
+        <v>260</v>
+      </c>
       <c r="H79" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I79" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
-      <c r="F80" t="s">
-        <v>182</v>
-      </c>
-      <c r="G80" s="1">
-        <v>56</v>
-      </c>
+      <c r="G80" s="10"/>
       <c r="H80" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I80" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="81" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
       <c r="F81" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G81" s="1">
         <v>56</v>
       </c>
       <c r="H81" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I81" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-      <c r="G82" s="10"/>
+      <c r="F82" t="s">
+        <v>183</v>
+      </c>
+      <c r="G82" s="1">
+        <v>56</v>
+      </c>
       <c r="H82" t="s">
-        <v>348</v>
+        <v>189</v>
       </c>
       <c r="I82" t="s">
-        <v>350</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="G83" s="1"/>
+      <c r="G83" s="10"/>
+      <c r="H83" t="s">
+        <v>348</v>
+      </c>
+      <c r="I83" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="84" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C85" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D84" s="1">
+      <c r="D85" s="1">
         <v>166</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E85" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F85" t="s">
         <v>194</v>
       </c>
-      <c r="G84" s="1">
+      <c r="G85" s="1">
         <v>50</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H85" t="s">
         <v>201</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I85" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="85" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F85" t="s">
-        <v>195</v>
-      </c>
-      <c r="G85" s="1">
-        <v>80</v>
-      </c>
-      <c r="H85" t="s">
-        <v>203</v>
-      </c>
-      <c r="I85" t="s">
-        <v>204</v>
-      </c>
-      <c r="N85" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="86" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
+      <c r="E86" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="F86" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G86" s="1">
         <v>80</v>
+      </c>
+      <c r="H86" t="s">
+        <v>203</v>
+      </c>
+      <c r="I86" t="s">
+        <v>204</v>
+      </c>
+      <c r="N86" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="87" spans="3:14" x14ac:dyDescent="0.3">
@@ -4073,7 +4109,7 @@
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G87" s="1">
         <v>80</v>
@@ -4084,19 +4120,10 @@
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G88" s="1">
-        <v>92</v>
-      </c>
-      <c r="H88" t="s">
-        <v>206</v>
-      </c>
-      <c r="I88" t="s">
-        <v>207</v>
-      </c>
-      <c r="N88" t="s">
-        <v>208</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="3:14" x14ac:dyDescent="0.3">
@@ -4104,10 +4131,19 @@
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G89" s="1">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="H89" t="s">
+        <v>206</v>
+      </c>
+      <c r="I89" t="s">
+        <v>207</v>
+      </c>
+      <c r="N89" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="90" spans="3:14" x14ac:dyDescent="0.3">
@@ -4115,28 +4151,27 @@
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G90" s="1">
-        <v>17</v>
-      </c>
-      <c r="H90" t="s">
-        <v>209</v>
-      </c>
-      <c r="I90" t="s">
-        <v>210</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
-      <c r="G91" s="10"/>
+      <c r="F91" t="s">
+        <v>200</v>
+      </c>
+      <c r="G91" s="1">
+        <v>17</v>
+      </c>
       <c r="H91" t="s">
-        <v>354</v>
+        <v>209</v>
       </c>
       <c r="I91" t="s">
-        <v>355</v>
+        <v>210</v>
       </c>
     </row>
     <row r="92" spans="3:14" x14ac:dyDescent="0.3">
@@ -4145,78 +4180,80 @@
       <c r="E92" s="1"/>
       <c r="G92" s="10"/>
       <c r="H92" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I92" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="93" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
+      <c r="G93" s="10"/>
+      <c r="H93" t="s">
+        <v>356</v>
+      </c>
+      <c r="I93" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="94" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C95" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D95" s="1">
         <v>176</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="E95" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F95" t="s">
         <v>212</v>
       </c>
-      <c r="G94" s="1">
+      <c r="G95" s="1">
         <v>50</v>
       </c>
-      <c r="H94" t="s">
+      <c r="H95" t="s">
         <v>201</v>
       </c>
-      <c r="I94" t="s">
+      <c r="I95" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="95" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F95" t="s">
-        <v>213</v>
-      </c>
-      <c r="G95" s="1">
-        <v>80</v>
-      </c>
-      <c r="H95" t="s">
-        <v>224</v>
-      </c>
-      <c r="I95" t="s">
-        <v>225</v>
-      </c>
-      <c r="N95" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="96" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
+      <c r="E96" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="F96" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G96" s="1">
         <v>80</v>
+      </c>
+      <c r="H96" t="s">
+        <v>224</v>
+      </c>
+      <c r="I96" t="s">
+        <v>225</v>
+      </c>
+      <c r="N96" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="97" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
       <c r="F97" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G97" s="1">
         <v>80</v>
@@ -4226,129 +4263,125 @@
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="F98" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G98" s="1">
-        <v>92</v>
-      </c>
-      <c r="H98" t="s">
-        <v>227</v>
-      </c>
-      <c r="I98" t="s">
-        <v>226</v>
-      </c>
-      <c r="N98" t="s">
-        <v>208</v>
+        <v>80</v>
       </c>
     </row>
     <row r="99" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="F99" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G99" s="1">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="H99" t="s">
+        <v>227</v>
+      </c>
+      <c r="I99" t="s">
+        <v>226</v>
+      </c>
+      <c r="N99" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="100" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="F100" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G100" s="1">
-        <v>17</v>
-      </c>
-      <c r="H100" t="s">
-        <v>219</v>
-      </c>
-      <c r="I100" t="s">
-        <v>223</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
+      <c r="F101" t="s">
+        <v>218</v>
+      </c>
+      <c r="G101" s="1">
+        <v>17</v>
+      </c>
+      <c r="H101" t="s">
+        <v>219</v>
+      </c>
+      <c r="I101" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="102" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+    </row>
+    <row r="103" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C103" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D102" s="1">
+      <c r="D103" s="1">
         <v>184</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="E103" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F103" t="s">
         <v>231</v>
       </c>
-      <c r="G102" s="1">
+      <c r="G103" s="1">
         <v>360</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H103" t="s">
         <v>236</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I103" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="103" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G103" s="10"/>
-      <c r="H103" t="s">
-        <v>253</v>
-      </c>
-      <c r="I103" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="104" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" t="s">
-        <v>230</v>
-      </c>
-      <c r="G104" s="1">
-        <v>440</v>
-      </c>
+      <c r="E104" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G104" s="10"/>
       <c r="H104" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I104" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
     </row>
     <row r="105" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
-      <c r="G105" s="10"/>
+      <c r="F105" t="s">
+        <v>230</v>
+      </c>
+      <c r="G105" s="1">
+        <v>440</v>
+      </c>
       <c r="H105" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="I105" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
     </row>
     <row r="106" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
-      <c r="F106" t="s">
-        <v>232</v>
-      </c>
-      <c r="G106" s="1">
-        <v>440</v>
+      <c r="G106" s="10"/>
+      <c r="H106" t="s">
+        <v>255</v>
       </c>
       <c r="I106" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
     </row>
     <row r="107" spans="3:16" x14ac:dyDescent="0.3">
@@ -4356,7 +4389,7 @@
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G107" s="1">
         <v>440</v>
@@ -4370,85 +4403,73 @@
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G108" s="1">
-        <v>20</v>
-      </c>
-      <c r="H108" s="2" t="s">
-        <v>243</v>
+        <v>440</v>
       </c>
       <c r="I108" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
       <c r="F109" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G109" s="1">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="I109" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
     </row>
     <row r="110" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
+      <c r="F110" t="s">
+        <v>235</v>
+      </c>
+      <c r="G110" s="1">
+        <v>80</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I110" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="111" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+    </row>
+    <row r="112" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C112" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D111" s="1">
+      <c r="D112" s="1">
         <v>190</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="E112" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F112" t="s">
         <v>246</v>
       </c>
-      <c r="G111" s="1">
+      <c r="G112" s="1">
         <v>3000</v>
       </c>
-      <c r="H111" t="s">
+      <c r="H112" t="s">
         <v>265</v>
       </c>
-      <c r="I111" s="3" t="s">
+      <c r="I112" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="J111" s="3"/>
-      <c r="K111" s="3"/>
-      <c r="L111" s="3"/>
-      <c r="M111" s="3"/>
-      <c r="N111" s="3"/>
-      <c r="O111" s="3"/>
-      <c r="P111" s="3"/>
-    </row>
-    <row r="112" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F112" t="s">
-        <v>247</v>
-      </c>
-      <c r="G112" s="1">
-        <v>2000</v>
-      </c>
-      <c r="H112" t="s">
-        <v>261</v>
-      </c>
-      <c r="I112" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="J112" s="3"/>
       <c r="K112" s="3"/>
@@ -4458,17 +4479,24 @@
       <c r="O112" s="3"/>
       <c r="P112" s="3"/>
     </row>
-    <row r="113" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
+      <c r="E113" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="F113" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G113" s="1">
         <v>2000</v>
       </c>
-      <c r="I113" s="3"/>
+      <c r="H113" t="s">
+        <v>261</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>262</v>
+      </c>
       <c r="J113" s="3"/>
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
@@ -4477,12 +4505,12 @@
       <c r="O113" s="3"/>
       <c r="P113" s="3"/>
     </row>
-    <row r="114" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G114" s="1">
         <v>2000</v>
@@ -4496,12 +4524,12 @@
       <c r="O114" s="3"/>
       <c r="P114" s="3"/>
     </row>
-    <row r="115" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G115" s="1">
         <v>2000</v>
@@ -4515,22 +4543,17 @@
       <c r="O115" s="3"/>
       <c r="P115" s="3"/>
     </row>
-    <row r="116" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G116" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H116" t="s">
-        <v>263</v>
-      </c>
-      <c r="I116" s="3" t="s">
-        <v>264</v>
-      </c>
+        <v>2000</v>
+      </c>
+      <c r="I116" s="3"/>
       <c r="J116" s="3"/>
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
@@ -4539,17 +4562,22 @@
       <c r="O116" s="3"/>
       <c r="P116" s="3"/>
     </row>
-    <row r="117" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G117" s="1">
         <v>1000</v>
       </c>
-      <c r="I117" s="3"/>
+      <c r="H117" t="s">
+        <v>263</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>264</v>
+      </c>
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
@@ -4558,11 +4586,16 @@
       <c r="O117" s="3"/>
       <c r="P117" s="3"/>
     </row>
-    <row r="118" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
-      <c r="G118" s="1"/>
+      <c r="F118" t="s">
+        <v>252</v>
+      </c>
+      <c r="G118" s="1">
+        <v>1000</v>
+      </c>
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
@@ -4572,26 +4605,12 @@
       <c r="O118" s="3"/>
       <c r="P118" s="3"/>
     </row>
-    <row r="119" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C119" s="1"/>
-      <c r="D119" s="1">
-        <v>172</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F119" t="s">
-        <v>274</v>
-      </c>
-      <c r="G119" s="1">
-        <v>50</v>
-      </c>
-      <c r="H119" t="s">
-        <v>280</v>
-      </c>
-      <c r="I119" s="3" t="s">
-        <v>281</v>
-      </c>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="I119" s="3"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
@@ -4600,23 +4619,25 @@
       <c r="O119" s="3"/>
       <c r="P119" s="3"/>
     </row>
-    <row r="120" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C120" s="1"/>
-      <c r="D120" s="1"/>
+      <c r="D120" s="1">
+        <v>172</v>
+      </c>
       <c r="E120" s="1" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="F120" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G120" s="1">
         <v>50</v>
       </c>
       <c r="H120" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="J120" s="3"/>
       <c r="K120" s="3"/>
@@ -4626,422 +4647,421 @@
       <c r="O120" s="3"/>
       <c r="P120" s="3"/>
     </row>
-    <row r="121" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
-      <c r="G121" s="1"/>
-    </row>
-    <row r="122" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="E121" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F121" t="s">
+        <v>275</v>
+      </c>
+      <c r="G121" s="1">
+        <v>50</v>
+      </c>
+      <c r="H121" t="s">
+        <v>284</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+      <c r="L121" s="3"/>
+      <c r="M121" s="3"/>
+      <c r="N121" s="3"/>
+      <c r="O121" s="3"/>
+      <c r="P121" s="3"/>
+    </row>
+    <row r="122" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
-      <c r="F122" t="s">
-        <v>276</v>
-      </c>
-      <c r="G122" s="1">
-        <v>65</v>
-      </c>
-      <c r="H122" t="s">
-        <v>292</v>
-      </c>
-      <c r="I122" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="123" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="G122" s="1"/>
+    </row>
+    <row r="123" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="F123" t="s">
-        <v>441</v>
+        <v>276</v>
       </c>
       <c r="G123" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H123" t="s">
-        <v>442</v>
-      </c>
-      <c r="I123" s="3" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="124" spans="3:18" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+      <c r="I123" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="124" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="F124" t="s">
-        <v>277</v>
+        <v>441</v>
       </c>
       <c r="G124" s="1">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="H124" t="s">
-        <v>293</v>
-      </c>
-      <c r="I124" t="s">
-        <v>413</v>
-      </c>
-      <c r="Q124" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="125" spans="3:18" x14ac:dyDescent="0.3">
+        <v>442</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="125" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="F125" t="s">
-        <v>431</v>
+        <v>277</v>
       </c>
       <c r="G125" s="1">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="126" spans="3:18" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="H125" t="s">
+        <v>293</v>
+      </c>
+      <c r="I125" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="126" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="F126" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G126" s="1">
-        <v>140</v>
-      </c>
-      <c r="H126" t="s">
-        <v>294</v>
-      </c>
-      <c r="I126" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="127" spans="3:18" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="127" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
+      <c r="F127" t="s">
+        <v>432</v>
+      </c>
+      <c r="G127" s="1">
+        <v>140</v>
+      </c>
       <c r="H127" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I127" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="128" spans="3:18" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="128" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
       <c r="H128" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I128" t="s">
-        <v>410</v>
-      </c>
-      <c r="R128" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="129" spans="3:9" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="129" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
-    </row>
-    <row r="130" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="H129" t="s">
+        <v>296</v>
+      </c>
+      <c r="I129" t="s">
+        <v>410</v>
+      </c>
+      <c r="R129" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="130" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
-      <c r="H130" t="s">
-        <v>291</v>
-      </c>
-      <c r="I130" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="131" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E130" s="1"/>
+    </row>
+    <row r="131" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="H131" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I131" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="132" spans="3:9" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="132" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="H132" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I132" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="133" spans="3:9" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="133" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
-      <c r="G133" s="1"/>
       <c r="H133" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="I133" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="134" spans="3:9" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="134" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="G134" s="1"/>
-    </row>
-    <row r="135" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="H134" t="s">
+        <v>286</v>
+      </c>
+      <c r="I134" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="135" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="G135" s="1"/>
-      <c r="H135" t="s">
-        <v>425</v>
-      </c>
-      <c r="I135" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="136" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="G136" s="1"/>
       <c r="H136" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I136" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="137" spans="3:9" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="137" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
-      <c r="F137" t="s">
-        <v>444</v>
-      </c>
-      <c r="G137" s="1">
-        <v>165</v>
-      </c>
+      <c r="G137" s="1"/>
       <c r="H137" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="I137" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="138" spans="3:9" x14ac:dyDescent="0.3">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="138" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="F138" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G138" s="1">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H138" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="I138" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="139" spans="3:9" x14ac:dyDescent="0.3">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="139" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="F139" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G139" s="1">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="H139" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I139" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="140" spans="3:9" x14ac:dyDescent="0.3">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="140" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
-      <c r="F140" t="s">
-        <v>449</v>
+      <c r="F140" s="11" t="s">
+        <v>448</v>
       </c>
       <c r="G140" s="1">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="H140" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="I140" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="141" spans="3:9" x14ac:dyDescent="0.3">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="141" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="F141" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="G141" s="1">
-        <v>280</v>
+        <v>210</v>
       </c>
       <c r="H141" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="I141" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="142" spans="3:9" x14ac:dyDescent="0.3">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="142" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="F142" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G142" s="1">
-        <v>500</v>
+        <v>280</v>
       </c>
       <c r="H142" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="I142" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="143" spans="3:9" x14ac:dyDescent="0.3">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="143" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
-      <c r="G143" s="1"/>
-    </row>
-    <row r="144" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F143" t="s">
+        <v>461</v>
+      </c>
+      <c r="G143" s="1">
+        <v>500</v>
+      </c>
+      <c r="H143" t="s">
+        <v>462</v>
+      </c>
+      <c r="I143" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="144" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
-      <c r="F144" t="s">
-        <v>278</v>
-      </c>
-      <c r="G144" s="1">
-        <v>60</v>
-      </c>
-      <c r="H144" s="2" t="s">
-        <v>297</v>
-      </c>
+      <c r="G144" s="1"/>
     </row>
     <row r="145" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
+      <c r="F145" t="s">
+        <v>278</v>
+      </c>
+      <c r="G145" s="1">
+        <v>60</v>
+      </c>
+      <c r="H145" s="2" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="146" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
-      <c r="F146" t="s">
-        <v>146</v>
-      </c>
-      <c r="G146" s="1">
-        <v>0</v>
-      </c>
-      <c r="H146" t="s">
-        <v>298</v>
-      </c>
-      <c r="I146" t="s">
-        <v>299</v>
-      </c>
     </row>
     <row r="147" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
       <c r="F147" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G147" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H147" t="s">
-        <v>219</v>
+        <v>298</v>
       </c>
       <c r="I147" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="148" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
-      <c r="E148" s="1"/>
       <c r="F148" t="s">
-        <v>279</v>
+        <v>145</v>
       </c>
       <c r="G148" s="1">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H148" t="s">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="I148" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
     </row>
     <row r="149" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
-      <c r="G149" s="1"/>
+      <c r="F149" t="s">
+        <v>279</v>
+      </c>
+      <c r="G149" s="1">
+        <v>11</v>
+      </c>
+      <c r="H149" t="s">
+        <v>282</v>
+      </c>
+      <c r="I149" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="150" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C150" s="1"/>
-      <c r="D150" s="1">
-        <v>180</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F150" t="s">
-        <v>301</v>
-      </c>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="G150" s="1"/>
     </row>
     <row r="151" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C151" s="1"/>
-      <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
-      <c r="G151" s="1"/>
-      <c r="I151" s="3"/>
+      <c r="D151" s="1">
+        <v>180</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F151" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="152" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="D152" s="1">
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="G152" s="1"/>
+      <c r="I152" s="3"/>
+    </row>
+    <row r="153" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="D153" s="1">
         <v>188</v>
       </c>
-      <c r="E152" s="1" t="s">
+      <c r="E153" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="F152" t="s">
+      <c r="F153" t="s">
         <v>304</v>
       </c>
-      <c r="G152" s="1">
+      <c r="G153" s="1">
         <v>400</v>
       </c>
-      <c r="H152" t="s">
+      <c r="H153" t="s">
         <v>312</v>
       </c>
-      <c r="I152" s="3" t="s">
+      <c r="I153" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="J152" s="3"/>
-      <c r="K152" s="3"/>
-      <c r="L152" s="3"/>
-      <c r="M152" s="3"/>
-      <c r="N152" s="3"/>
-      <c r="O152" s="3"/>
-      <c r="P152" s="3"/>
-      <c r="Q152" s="3"/>
-    </row>
-    <row r="153" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C153" s="1"/>
-      <c r="D153" s="1"/>
-      <c r="E153" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F153" t="s">
-        <v>305</v>
-      </c>
-      <c r="G153" s="1">
-        <v>12000</v>
-      </c>
-      <c r="H153" t="s">
-        <v>318</v>
-      </c>
-      <c r="I153" s="3" t="s">
-        <v>319</v>
       </c>
       <c r="J153" s="3"/>
       <c r="K153" s="3"/>
@@ -5055,17 +5075,20 @@
     <row r="154" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
+      <c r="E154" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="F154" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G154" s="1">
-        <v>400</v>
+        <v>12000</v>
       </c>
       <c r="H154" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="I154" s="3" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="J154" s="3"/>
       <c r="K154" s="3"/>
@@ -5079,12 +5102,17 @@
     <row r="155" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
-      <c r="G155" s="1"/>
+      <c r="F155" t="s">
+        <v>306</v>
+      </c>
+      <c r="G155" s="1">
+        <v>400</v>
+      </c>
       <c r="H155" t="s">
-        <v>241</v>
+        <v>316</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>434</v>
+        <v>317</v>
       </c>
       <c r="J155" s="3"/>
       <c r="K155" s="3"/>
@@ -5098,11 +5126,12 @@
     <row r="156" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
+      <c r="G156" s="1"/>
       <c r="H156" t="s">
         <v>241</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
@@ -5116,18 +5145,13 @@
     <row r="157" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
-      <c r="F157" t="s">
-        <v>307</v>
-      </c>
-      <c r="G157" s="1">
-        <v>800</v>
-      </c>
       <c r="H157" t="s">
-        <v>439</v>
+        <v>241</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>440</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="J157" s="3"/>
       <c r="K157" s="3"/>
       <c r="L157" s="3"/>
       <c r="M157" s="3"/>
@@ -5139,14 +5163,18 @@
     <row r="158" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
-      <c r="G158" s="1"/>
+      <c r="F158" t="s">
+        <v>307</v>
+      </c>
+      <c r="G158" s="1">
+        <v>800</v>
+      </c>
       <c r="H158" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="J158" s="3"/>
+        <v>440</v>
+      </c>
       <c r="K158" s="3"/>
       <c r="L158" s="3"/>
       <c r="M158" s="3"/>
@@ -5158,17 +5186,12 @@
     <row r="159" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
-      <c r="F159" t="s">
-        <v>308</v>
-      </c>
-      <c r="G159" s="1">
-        <v>1600</v>
-      </c>
+      <c r="G159" s="1"/>
       <c r="H159" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="J159" s="3"/>
       <c r="K159" s="3"/>
@@ -5182,8 +5205,18 @@
     <row r="160" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
-      <c r="G160" s="1"/>
-      <c r="I160" s="3"/>
+      <c r="F160" t="s">
+        <v>308</v>
+      </c>
+      <c r="G160" s="1">
+        <v>1600</v>
+      </c>
+      <c r="H160" t="s">
+        <v>436</v>
+      </c>
+      <c r="I160" s="3" t="s">
+        <v>435</v>
+      </c>
       <c r="J160" s="3"/>
       <c r="K160" s="3"/>
       <c r="L160" s="3"/>
@@ -5196,18 +5229,8 @@
     <row r="161" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
-      <c r="F161" t="s">
-        <v>309</v>
-      </c>
-      <c r="G161" s="1">
-        <v>20</v>
-      </c>
-      <c r="H161" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="I161" t="s">
-        <v>244</v>
-      </c>
+      <c r="G161" s="1"/>
+      <c r="I161" s="3"/>
       <c r="J161" s="3"/>
       <c r="K161" s="3"/>
       <c r="L161" s="3"/>
@@ -5221,16 +5244,16 @@
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
       <c r="F162" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G162" s="1">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="I162" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="J162" s="3"/>
       <c r="K162" s="3"/>
@@ -5245,16 +5268,16 @@
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
       <c r="F163" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G163" s="1">
-        <v>480</v>
-      </c>
-      <c r="H163" t="s">
-        <v>313</v>
-      </c>
-      <c r="I163" s="3" t="s">
-        <v>315</v>
+        <v>80</v>
+      </c>
+      <c r="H163" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I163" t="s">
+        <v>258</v>
       </c>
       <c r="J163" s="3"/>
       <c r="K163" s="3"/>
@@ -5268,9 +5291,18 @@
     <row r="164" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
-      <c r="E164" s="1"/>
-      <c r="G164" s="1"/>
-      <c r="I164" s="3"/>
+      <c r="F164" t="s">
+        <v>311</v>
+      </c>
+      <c r="G164" s="1">
+        <v>480</v>
+      </c>
+      <c r="H164" t="s">
+        <v>313</v>
+      </c>
+      <c r="I164" s="3" t="s">
+        <v>315</v>
+      </c>
       <c r="J164" s="3"/>
       <c r="K164" s="3"/>
       <c r="L164" s="3"/>
@@ -5297,24 +5329,10 @@
     </row>
     <row r="166" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C166" s="1"/>
-      <c r="D166" s="1">
-        <v>194</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F166" t="s">
-        <v>321</v>
-      </c>
-      <c r="G166" s="1">
-        <v>4000</v>
-      </c>
-      <c r="H166" t="s">
-        <v>329</v>
-      </c>
-      <c r="I166" s="3" t="s">
-        <v>330</v>
-      </c>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="G166" s="1"/>
+      <c r="I166" s="3"/>
       <c r="J166" s="3"/>
       <c r="K166" s="3"/>
       <c r="L166" s="3"/>
@@ -5326,15 +5344,24 @@
     </row>
     <row r="167" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
-      <c r="E167" s="1"/>
+      <c r="D167" s="1">
+        <v>194</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="F167" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G167" s="1">
-        <v>12000</v>
-      </c>
-      <c r="I167" s="3"/>
+        <v>4000</v>
+      </c>
+      <c r="H167" t="s">
+        <v>329</v>
+      </c>
+      <c r="I167" s="3" t="s">
+        <v>330</v>
+      </c>
       <c r="J167" s="3"/>
       <c r="K167" s="3"/>
       <c r="L167" s="3"/>
@@ -5349,17 +5376,12 @@
       <c r="D168" s="1"/>
       <c r="E168" s="1"/>
       <c r="F168" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G168" s="1">
-        <v>2000</v>
-      </c>
-      <c r="H168" t="s">
-        <v>331</v>
-      </c>
-      <c r="I168" s="3" t="s">
-        <v>332</v>
-      </c>
+        <v>12000</v>
+      </c>
+      <c r="I168" s="3"/>
       <c r="J168" s="3"/>
       <c r="K168" s="3"/>
       <c r="L168" s="3"/>
@@ -5374,15 +5396,17 @@
       <c r="D169" s="1"/>
       <c r="E169" s="1"/>
       <c r="F169" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G169" s="1">
         <v>2000</v>
       </c>
       <c r="H169" t="s">
-        <v>241</v>
-      </c>
-      <c r="I169" s="3"/>
+        <v>331</v>
+      </c>
+      <c r="I169" s="3" t="s">
+        <v>332</v>
+      </c>
       <c r="J169" s="3"/>
       <c r="K169" s="3"/>
       <c r="L169" s="3"/>
@@ -5397,7 +5421,7 @@
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
       <c r="F170" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G170" s="1">
         <v>2000</v>
@@ -5419,7 +5443,15 @@
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
-      <c r="G171" s="1"/>
+      <c r="F171" t="s">
+        <v>325</v>
+      </c>
+      <c r="G171" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H171" t="s">
+        <v>241</v>
+      </c>
       <c r="I171" s="3"/>
       <c r="J171" s="3"/>
       <c r="K171" s="3"/>
@@ -5434,18 +5466,8 @@
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
-      <c r="F172" t="s">
-        <v>326</v>
-      </c>
-      <c r="G172" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H172" t="s">
-        <v>263</v>
-      </c>
-      <c r="I172" s="3" t="s">
-        <v>264</v>
-      </c>
+      <c r="G172" s="1"/>
+      <c r="I172" s="3"/>
       <c r="J172" s="3"/>
       <c r="K172" s="3"/>
       <c r="L172" s="3"/>
@@ -5460,12 +5482,17 @@
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
       <c r="F173" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G173" s="1">
         <v>1000</v>
       </c>
-      <c r="I173" s="3"/>
+      <c r="H173" t="s">
+        <v>263</v>
+      </c>
+      <c r="I173" s="3" t="s">
+        <v>264</v>
+      </c>
       <c r="J173" s="3"/>
       <c r="K173" s="3"/>
       <c r="L173" s="3"/>
@@ -5479,7 +5506,12 @@
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
-      <c r="G174" s="1"/>
+      <c r="F174" t="s">
+        <v>327</v>
+      </c>
+      <c r="G174" s="1">
+        <v>1000</v>
+      </c>
       <c r="I174" s="3"/>
       <c r="J174" s="3"/>
       <c r="K174" s="3"/>
@@ -5494,15 +5526,7 @@
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
-      <c r="F175" t="s">
-        <v>328</v>
-      </c>
-      <c r="G175" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="H175" t="s">
-        <v>241</v>
-      </c>
+      <c r="G175" s="1"/>
       <c r="I175" s="3"/>
       <c r="J175" s="3"/>
       <c r="K175" s="3"/>
@@ -5517,7 +5541,15 @@
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
-      <c r="G176" s="1"/>
+      <c r="F176" t="s">
+        <v>328</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H176" t="s">
+        <v>241</v>
+      </c>
       <c r="I176" s="3"/>
       <c r="J176" s="3"/>
       <c r="K176" s="3"/>
@@ -5528,136 +5560,147 @@
       <c r="P176" s="3"/>
       <c r="Q176" s="3"/>
     </row>
-    <row r="177" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
-      <c r="E177" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F177" t="s">
-        <v>334</v>
-      </c>
-      <c r="G177" s="1">
-        <v>170</v>
-      </c>
-      <c r="H177" t="s">
-        <v>335</v>
-      </c>
-      <c r="I177" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="178" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="E177" s="1"/>
+      <c r="G177" s="1"/>
+      <c r="I177" s="3"/>
+      <c r="J177" s="3"/>
+      <c r="K177" s="3"/>
+      <c r="L177" s="3"/>
+      <c r="M177" s="3"/>
+      <c r="N177" s="3"/>
+      <c r="O177" s="3"/>
+      <c r="P177" s="3"/>
+      <c r="Q177" s="3"/>
+    </row>
+    <row r="178" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
-      <c r="E178" s="1"/>
+      <c r="E178" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="F178" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="G178" s="1">
         <v>170</v>
       </c>
       <c r="H178" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="I178" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="179" spans="3:9" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="179" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
       <c r="F179" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="G179" s="1">
-        <v>95</v>
+        <v>170</v>
       </c>
       <c r="H179" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="I179" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="180" spans="3:9" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="180" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
       <c r="E180" s="1"/>
       <c r="F180" t="s">
+        <v>337</v>
+      </c>
+      <c r="G180" s="1">
+        <v>95</v>
+      </c>
+      <c r="H180" t="s">
+        <v>338</v>
+      </c>
+      <c r="I180" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="181" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" t="s">
         <v>456</v>
       </c>
-      <c r="G180" s="1">
+      <c r="G181" s="1">
         <v>160000</v>
       </c>
-      <c r="H180" t="s">
+      <c r="H181" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="181" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C181" s="9"/>
-      <c r="D181" s="1"/>
-      <c r="E181" s="1" t="s">
+    <row r="182" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C182" s="9"/>
+      <c r="D182" s="1"/>
+      <c r="E182" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="F181" t="s">
+      <c r="F182" t="s">
         <v>386</v>
       </c>
-      <c r="H181" t="s">
+      <c r="H182" t="s">
         <v>387</v>
       </c>
-      <c r="I181" t="s">
+      <c r="I182" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="182" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C182" s="1"/>
-      <c r="D182" s="1"/>
-    </row>
-    <row r="183" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
-      <c r="H183" t="s">
-        <v>343</v>
-      </c>
-      <c r="I183" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="184" spans="3:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="184" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
-    </row>
-    <row r="185" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="H184" t="s">
+        <v>343</v>
+      </c>
+      <c r="I184" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="185" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
     </row>
-    <row r="186" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
     </row>
-    <row r="187" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
     </row>
-    <row r="188" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
     </row>
-    <row r="189" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
     </row>
-    <row r="190" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
     </row>
-    <row r="191" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
     </row>
-    <row r="192" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
     </row>
@@ -5670,6 +5713,7 @@
       <c r="D194" s="1"/>
     </row>
     <row r="195" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C195" s="1"/>
       <c r="D195" s="1"/>
     </row>
     <row r="196" spans="3:4" x14ac:dyDescent="0.3">
@@ -5704,6 +5748,9 @@
     </row>
     <row r="206" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D206" s="1"/>
+    </row>
+    <row r="207" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D207" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Delete spaces between Layer figure
</commit_message>
<xml_diff>
--- a/28nm_DRC_Layer.xlsx
+++ b/28nm_DRC_Layer.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://postechackr-my.sharepoint.com/personal/junung_postech_ac_kr/Documents/연구/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iksu Jang\Desktop\Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{2D172E4F-C5BA-424F-896E-5EE36FD45D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{462F7C80-D1C2-4A56-97E7-2BD13CA8C48F}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1530" windowWidth="24300" windowHeight="12765" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="1530" windowWidth="24300" windowHeight="12765" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1897,7 +1896,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2016,7 +2015,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2039,9 +2038,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1">
@@ -2337,7 +2333,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E3:U44"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -2881,11 +2877,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AA207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3012,20 +3008,24 @@
       <c r="G11" s="1">
         <v>240</v>
       </c>
-      <c r="S11" s="8"/>
+      <c r="S11" s="1" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="G12" s="10"/>
+      <c r="G12" s="9"/>
       <c r="H12" t="s">
         <v>345</v>
       </c>
       <c r="I12" t="s">
         <v>88</v>
       </c>
-      <c r="S12" s="8"/>
+      <c r="S12" s="4" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
@@ -3034,7 +3034,7 @@
       <c r="F13" t="s">
         <v>464</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="11">
         <v>160000</v>
       </c>
       <c r="H13" t="s">
@@ -3043,15 +3043,17 @@
       <c r="I13" t="s">
         <v>466</v>
       </c>
-      <c r="S13" s="8"/>
+      <c r="S13" s="1" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="S14" s="1" t="s">
-        <v>260</v>
+      <c r="S14" s="4" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.3">
@@ -3073,8 +3075,8 @@
       <c r="I15" t="s">
         <v>393</v>
       </c>
-      <c r="S15" s="4" t="s">
-        <v>359</v>
+      <c r="S15" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.3">
@@ -3090,8 +3092,8 @@
       <c r="I16" t="s">
         <v>394</v>
       </c>
-      <c r="S16" s="1" t="s">
-        <v>360</v>
+      <c r="S16" s="4" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="17" spans="3:27" x14ac:dyDescent="0.3">
@@ -3101,90 +3103,90 @@
       <c r="F17" t="s">
         <v>395</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="9"/>
       <c r="H17" t="s">
         <v>100</v>
       </c>
       <c r="I17" t="s">
         <v>101</v>
       </c>
-      <c r="S17" s="4" t="s">
-        <v>361</v>
+      <c r="S17" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="G18" s="10"/>
+      <c r="G18" s="9"/>
       <c r="H18" t="s">
         <v>96</v>
       </c>
       <c r="I18" t="s">
         <v>97</v>
       </c>
-      <c r="S18" s="1" t="s">
-        <v>242</v>
+      <c r="S18" s="4" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="G19" s="10"/>
+      <c r="G19" s="9"/>
       <c r="H19" t="s">
         <v>351</v>
       </c>
       <c r="I19" t="s">
         <v>352</v>
       </c>
-      <c r="S19" s="4" t="s">
-        <v>362</v>
+      <c r="S19" s="1" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="G20" s="10"/>
+      <c r="G20" s="9"/>
       <c r="H20" t="s">
         <v>351</v>
       </c>
       <c r="I20" t="s">
         <v>353</v>
       </c>
-      <c r="S20" s="1" t="s">
-        <v>363</v>
+      <c r="S20" s="4" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="G21" s="10"/>
+      <c r="G21" s="9"/>
       <c r="H21" t="s">
         <v>389</v>
       </c>
       <c r="I21" t="s">
         <v>390</v>
       </c>
-      <c r="S21" s="4" t="s">
-        <v>364</v>
+      <c r="S21" s="1" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="22" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="G22" s="10"/>
+      <c r="G22" s="9"/>
       <c r="H22" t="s">
         <v>391</v>
       </c>
       <c r="I22" t="s">
         <v>392</v>
       </c>
-      <c r="S22" s="1" t="s">
-        <v>365</v>
+      <c r="S22" s="4" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="23" spans="3:27" x14ac:dyDescent="0.3">
@@ -3192,8 +3194,8 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="S23" s="4" t="s">
-        <v>366</v>
+      <c r="S23" s="1" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="24" spans="3:27" x14ac:dyDescent="0.3">
@@ -3218,8 +3220,8 @@
       <c r="I24" t="s">
         <v>108</v>
       </c>
-      <c r="S24" s="1" t="s">
-        <v>367</v>
+      <c r="S24" s="4" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="3:27" x14ac:dyDescent="0.3">
@@ -3237,8 +3239,8 @@
       <c r="I25" t="s">
         <v>110</v>
       </c>
-      <c r="S25" s="4" t="s">
-        <v>368</v>
+      <c r="S25" s="1" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="3:27" x14ac:dyDescent="0.3">
@@ -3250,8 +3252,8 @@
       <c r="G26" s="1">
         <v>96</v>
       </c>
-      <c r="S26" s="1" t="s">
-        <v>369</v>
+      <c r="S26" s="4" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="3:27" x14ac:dyDescent="0.3">
@@ -3269,11 +3271,13 @@
       <c r="I27" t="s">
         <v>112</v>
       </c>
-      <c r="S27" s="4" t="s">
-        <v>370</v>
+      <c r="S27" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="AA27" s="1"/>
     </row>
     <row r="28" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
@@ -3290,11 +3294,21 @@
       <c r="I28" t="s">
         <v>114</v>
       </c>
-      <c r="S28" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
+      <c r="S28" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="U28" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="W28" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="Y28" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="AA28" s="4" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="29" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
@@ -3308,12 +3322,21 @@
       <c r="I29" t="s">
         <v>110</v>
       </c>
-      <c r="S29" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="Y29" s="1"/>
+      <c r="S29" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="30" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
@@ -3324,10 +3347,21 @@
       <c r="G30" s="1">
         <v>96</v>
       </c>
-      <c r="S30" s="8"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="Y30" s="1"/>
+      <c r="S30" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="U30" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="W30" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="Y30" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="AA30" s="4" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="31" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
@@ -3338,8 +3372,8 @@
       <c r="G31" s="1">
         <v>96</v>
       </c>
-      <c r="S31" s="8"/>
-      <c r="U31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="U31" s="5"/>
       <c r="V31" s="1"/>
       <c r="Y31" s="1"/>
     </row>
@@ -3353,35 +3387,29 @@
       <c r="I32" t="s">
         <v>347</v>
       </c>
-      <c r="S32" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="U32" s="1"/>
+      <c r="S32" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="U32" s="6" t="s">
+        <v>378</v>
+      </c>
       <c r="V32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="AA32" s="1"/>
-    </row>
-    <row r="33" spans="3:27" x14ac:dyDescent="0.3">
+      <c r="W32" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="Y32" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="AA32" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="33" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="S33" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="U33" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="W33" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="Y33" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="AA33" s="4" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="34" spans="3:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>404</v>
       </c>
@@ -3400,23 +3428,8 @@
       <c r="I34" t="s">
         <v>125</v>
       </c>
-      <c r="S34" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="W34" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="Y34" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="AA34" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="35" spans="3:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="F35" t="s">
@@ -3434,23 +3447,8 @@
       <c r="N35" t="s">
         <v>240</v>
       </c>
-      <c r="S35" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="U35" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="W35" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="Y35" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="AA35" s="4" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="36" spans="3:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="F36" t="s">
@@ -3459,12 +3457,8 @@
       <c r="G36" s="1">
         <v>60</v>
       </c>
-      <c r="S36" s="1"/>
-      <c r="U36" s="5"/>
-      <c r="V36" s="1"/>
-      <c r="Y36" s="1"/>
-    </row>
-    <row r="37" spans="3:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="F37" t="s">
@@ -3479,24 +3473,8 @@
       <c r="I37" t="s">
         <v>129</v>
       </c>
-      <c r="S37" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="U37" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="V37" s="1"/>
-      <c r="W37" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y37" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="AA37" s="6" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="38" spans="3:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="F38" t="s">
@@ -3509,7 +3487,7 @@
       <c r="V38" s="1"/>
       <c r="Y38" s="1"/>
     </row>
-    <row r="39" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="F39" t="s">
@@ -3526,7 +3504,7 @@
       </c>
       <c r="Y39" s="1"/>
     </row>
-    <row r="40" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="F40" t="s">
@@ -3542,10 +3520,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="G41" s="10"/>
+      <c r="G41" s="9"/>
       <c r="H41" t="s">
         <v>134</v>
       </c>
@@ -3553,7 +3531,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="F42" t="s">
@@ -3569,7 +3547,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="F43" t="s">
@@ -3579,10 +3557,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="G44" s="10"/>
+      <c r="G44" s="9"/>
       <c r="H44" t="s">
         <v>383</v>
       </c>
@@ -3590,12 +3568,12 @@
         <v>384</v>
       </c>
     </row>
-    <row r="45" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C46" s="1" t="s">
         <v>15</v>
       </c>
@@ -3618,7 +3596,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="47" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="F47" t="s">
@@ -3634,7 +3612,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="G48" s="1"/>
@@ -3674,7 +3652,7 @@
     <row r="51" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="10" t="s">
         <v>142</v>
       </c>
       <c r="G51" s="1">
@@ -3684,7 +3662,7 @@
     <row r="52" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="10" t="s">
         <v>143</v>
       </c>
       <c r="G52" s="1">
@@ -4000,7 +3978,7 @@
     <row r="80" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
-      <c r="G80" s="10"/>
+      <c r="G80" s="9"/>
       <c r="H80" t="s">
         <v>187</v>
       </c>
@@ -4045,7 +4023,7 @@
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="G83" s="10"/>
+      <c r="G83" s="9"/>
       <c r="H83" t="s">
         <v>348</v>
       </c>
@@ -4178,7 +4156,7 @@
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
-      <c r="G92" s="10"/>
+      <c r="G92" s="9"/>
       <c r="H92" t="s">
         <v>354</v>
       </c>
@@ -4190,7 +4168,7 @@
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
-      <c r="G93" s="10"/>
+      <c r="G93" s="9"/>
       <c r="H93" t="s">
         <v>356</v>
       </c>
@@ -4347,7 +4325,7 @@
       <c r="E104" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="G104" s="10"/>
+      <c r="G104" s="9"/>
       <c r="H104" t="s">
         <v>253</v>
       </c>
@@ -4376,7 +4354,7 @@
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
-      <c r="G106" s="10"/>
+      <c r="G106" s="9"/>
       <c r="H106" t="s">
         <v>255</v>
       </c>
@@ -4887,7 +4865,7 @@
     <row r="140" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
-      <c r="F140" s="11" t="s">
+      <c r="F140" s="10" t="s">
         <v>448</v>
       </c>
       <c r="G140" s="1">
@@ -5643,7 +5621,7 @@
       </c>
     </row>
     <row r="182" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C182" s="9"/>
+      <c r="C182" s="8"/>
       <c r="D182" s="1"/>
       <c r="E182" s="1" t="s">
         <v>385</v>

</xml_diff>

<commit_message>
Add description of GR502a
</commit_message>
<xml_diff>
--- a/28nm_DRC_Layer.xlsx
+++ b/28nm_DRC_Layer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iksu Jang\Desktop\Playground\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Germanus\Documents\GitHub\Playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="468">
   <si>
     <t>65nm</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1891,13 +1891,56 @@
   </si>
   <si>
     <t>PH (as generated by Boolean) minimum enclosed area (um2) &gt;= 0.16</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">At GR502a1, (M1 or (size edge (M1_end with edge length &lt; 0.058 um) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>outside by 0.010 um</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) or (size edge (M1_end with edge length &gt;= 0.058 um) outside by 0.006 um)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>minimum space and notch &gt;= 0.05</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1945,6 +1988,16 @@
       <color rgb="FF9C0006"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -2880,8 +2933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AA207"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U58" sqref="U58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3792,7 +3845,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="G65" s="1"/>
@@ -3803,12 +3856,12 @@
         <v>422</v>
       </c>
     </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="F67" t="s">
@@ -3823,8 +3876,11 @@
       <c r="I67" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="J67" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="F68" t="s">
@@ -3837,7 +3893,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="F69" t="s">
@@ -3853,7 +3909,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="G70" s="1"/>
@@ -3864,7 +3920,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="G71" s="1"/>
@@ -3875,12 +3931,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="F73" t="s">
@@ -3894,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="F74" t="s">
@@ -3910,12 +3966,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="F76" t="s">
@@ -3931,12 +3987,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C78" s="1" t="s">
         <v>423</v>
       </c>
@@ -3959,7 +4015,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="F79" t="s">
@@ -3975,7 +4031,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="80" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="G80" s="9"/>

</xml_diff>

<commit_message>
Fix typo and Add some Layers
- Fix : @ DRC, SLVT minimum area
- Add : @ DesignParameters.py, LVT HVT layers
</commit_message>
<xml_diff>
--- a/28nm_DRC_Layer.xlsx
+++ b/28nm_DRC_Layer.xlsx
@@ -1385,10 +1385,6 @@
   </si>
   <si>
     <t>SlvtMinArea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GRSLVT1_noNW</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1933,6 +1929,10 @@
       </rPr>
       <t>minimum space and notch &gt;= 0.05</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GRSLVT10_noNW</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2933,8 +2933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AA207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U58" sqref="U58"/>
+    <sheetView tabSelected="1" topLeftCell="B154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J186" sqref="J186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>179</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D7" s="1">
         <v>146</v>
@@ -3042,13 +3042,13 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G10" s="1">
         <v>132</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.3">
@@ -3056,7 +3056,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G11" s="1">
         <v>240</v>
@@ -3071,13 +3071,13 @@
       <c r="E12" s="1"/>
       <c r="G12" s="9"/>
       <c r="H12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I12" t="s">
         <v>88</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.3">
@@ -3085,19 +3085,19 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G13" s="11">
         <v>160000</v>
       </c>
       <c r="H13" t="s">
+        <v>464</v>
+      </c>
+      <c r="I13" t="s">
         <v>465</v>
       </c>
-      <c r="I13" t="s">
-        <v>466</v>
-      </c>
       <c r="S13" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.3">
@@ -3106,12 +3106,12 @@
       <c r="E14" s="1"/>
       <c r="G14" s="1"/>
       <c r="S14" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D15" s="1">
         <v>107</v>
@@ -3126,7 +3126,7 @@
         <v>140</v>
       </c>
       <c r="I15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>242</v>
@@ -3143,10 +3143,10 @@
         <v>70</v>
       </c>
       <c r="I16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17" spans="3:27" x14ac:dyDescent="0.3">
@@ -3154,7 +3154,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" t="s">
@@ -3164,7 +3164,7 @@
         <v>101</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="3:27" x14ac:dyDescent="0.3">
@@ -3179,7 +3179,7 @@
         <v>97</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" spans="3:27" x14ac:dyDescent="0.3">
@@ -3188,13 +3188,13 @@
       <c r="E19" s="1"/>
       <c r="G19" s="9"/>
       <c r="H19" t="s">
+        <v>350</v>
+      </c>
+      <c r="I19" t="s">
         <v>351</v>
       </c>
-      <c r="I19" t="s">
-        <v>352</v>
-      </c>
       <c r="S19" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="20" spans="3:27" x14ac:dyDescent="0.3">
@@ -3203,13 +3203,13 @@
       <c r="E20" s="1"/>
       <c r="G20" s="9"/>
       <c r="H20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="3:27" x14ac:dyDescent="0.3">
@@ -3218,13 +3218,13 @@
       <c r="E21" s="1"/>
       <c r="G21" s="9"/>
       <c r="H21" t="s">
+        <v>388</v>
+      </c>
+      <c r="I21" t="s">
         <v>389</v>
       </c>
-      <c r="I21" t="s">
-        <v>390</v>
-      </c>
       <c r="S21" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22" spans="3:27" x14ac:dyDescent="0.3">
@@ -3233,13 +3233,13 @@
       <c r="E22" s="1"/>
       <c r="G22" s="9"/>
       <c r="H22" t="s">
+        <v>390</v>
+      </c>
+      <c r="I22" t="s">
         <v>391</v>
       </c>
-      <c r="I22" t="s">
-        <v>392</v>
-      </c>
       <c r="S22" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="23" spans="3:27" x14ac:dyDescent="0.3">
@@ -3248,12 +3248,12 @@
       <c r="E23" s="1"/>
       <c r="G23" s="1"/>
       <c r="S23" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="24" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D24" s="1">
         <v>123</v>
@@ -3274,7 +3274,7 @@
         <v>108</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="25" spans="3:27" x14ac:dyDescent="0.3">
@@ -3306,7 +3306,7 @@
         <v>96</v>
       </c>
       <c r="S26" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="3:27" x14ac:dyDescent="0.3">
@@ -3348,19 +3348,19 @@
         <v>114</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="U28" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AA28" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="29" spans="3:27" x14ac:dyDescent="0.3">
@@ -3376,51 +3376,51 @@
         <v>110</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AA29" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="30" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="F30" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G30" s="1">
         <v>96</v>
       </c>
       <c r="S30" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="U30" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="W30" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="Y30" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="AA30" s="4" t="s">
         <v>374</v>
-      </c>
-      <c r="U30" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="W30" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="Y30" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="AA30" s="4" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="31" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="F31" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G31" s="1">
         <v>96</v>
@@ -3435,26 +3435,26 @@
       <c r="D32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
+        <v>345</v>
+      </c>
+      <c r="I32" t="s">
         <v>346</v>
       </c>
-      <c r="I32" t="s">
-        <v>347</v>
-      </c>
       <c r="S32" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="U32" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="V32" s="1"/>
       <c r="W32" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="Y32" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="Y32" s="6" t="s">
+      <c r="AA32" s="6" t="s">
         <v>380</v>
-      </c>
-      <c r="AA32" s="6" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="33" spans="3:25" x14ac:dyDescent="0.3">
@@ -3464,7 +3464,7 @@
     </row>
     <row r="34" spans="3:25" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D34" s="1">
         <v>158</v>
@@ -3615,10 +3615,10 @@
       <c r="D44" s="1"/>
       <c r="G44" s="9"/>
       <c r="H44" t="s">
+        <v>382</v>
+      </c>
+      <c r="I44" t="s">
         <v>383</v>
-      </c>
-      <c r="I44" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="45" spans="3:25" x14ac:dyDescent="0.3">
@@ -3683,7 +3683,7 @@
         <v>167</v>
       </c>
       <c r="I49" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="50" spans="3:16" x14ac:dyDescent="0.3">
@@ -3699,7 +3699,7 @@
         <v>156</v>
       </c>
       <c r="I50" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="51" spans="3:16" x14ac:dyDescent="0.3">
@@ -3725,7 +3725,7 @@
         <v>288</v>
       </c>
       <c r="I52" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="53" spans="3:16" x14ac:dyDescent="0.3">
@@ -3736,7 +3736,7 @@
         <v>165</v>
       </c>
       <c r="I53" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="54" spans="3:16" x14ac:dyDescent="0.3">
@@ -3747,7 +3747,7 @@
         <v>157</v>
       </c>
       <c r="I54" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="55" spans="3:16" x14ac:dyDescent="0.3">
@@ -3763,7 +3763,7 @@
         <v>158</v>
       </c>
       <c r="I56" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="57" spans="3:16" x14ac:dyDescent="0.3">
@@ -3774,7 +3774,7 @@
         <v>163</v>
       </c>
       <c r="I57" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="58" spans="3:16" x14ac:dyDescent="0.3">
@@ -3785,7 +3785,7 @@
         <v>160</v>
       </c>
       <c r="I58" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="59" spans="3:16" x14ac:dyDescent="0.3">
@@ -3796,10 +3796,10 @@
         <v>159</v>
       </c>
       <c r="I59" t="s">
+        <v>404</v>
+      </c>
+      <c r="P59" t="s">
         <v>405</v>
-      </c>
-      <c r="P59" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="60" spans="3:16" x14ac:dyDescent="0.3">
@@ -3812,10 +3812,10 @@
       <c r="D61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
+        <v>414</v>
+      </c>
+      <c r="I61" t="s">
         <v>415</v>
-      </c>
-      <c r="I61" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="62" spans="3:16" x14ac:dyDescent="0.3">
@@ -3823,10 +3823,10 @@
       <c r="D62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" t="s">
+        <v>416</v>
+      </c>
+      <c r="I62" t="s">
         <v>417</v>
-      </c>
-      <c r="I62" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="63" spans="3:16" x14ac:dyDescent="0.3">
@@ -3839,10 +3839,10 @@
       <c r="D64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" t="s">
+        <v>418</v>
+      </c>
+      <c r="I64" t="s">
         <v>419</v>
-      </c>
-      <c r="I64" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="65" spans="3:10" x14ac:dyDescent="0.3">
@@ -3850,10 +3850,10 @@
       <c r="D65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" t="s">
+        <v>420</v>
+      </c>
+      <c r="I65" t="s">
         <v>421</v>
-      </c>
-      <c r="I65" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="66" spans="3:10" x14ac:dyDescent="0.3">
@@ -3877,7 +3877,7 @@
         <v>169</v>
       </c>
       <c r="J67" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="68" spans="3:10" x14ac:dyDescent="0.3">
@@ -3994,7 +3994,7 @@
     </row>
     <row r="78" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C78" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D78" s="1">
         <v>110</v>
@@ -4009,7 +4009,7 @@
         <v>260</v>
       </c>
       <c r="H78" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I78" t="s">
         <v>184</v>
@@ -4081,10 +4081,10 @@
       <c r="E83" s="1"/>
       <c r="G83" s="9"/>
       <c r="H83" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I83" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="84" spans="3:14" x14ac:dyDescent="0.3">
@@ -4214,10 +4214,10 @@
       <c r="E92" s="1"/>
       <c r="G92" s="9"/>
       <c r="H92" t="s">
+        <v>353</v>
+      </c>
+      <c r="I92" t="s">
         <v>354</v>
-      </c>
-      <c r="I92" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="93" spans="3:14" x14ac:dyDescent="0.3">
@@ -4226,10 +4226,10 @@
       <c r="E93" s="1"/>
       <c r="G93" s="9"/>
       <c r="H93" t="s">
+        <v>355</v>
+      </c>
+      <c r="I93" t="s">
         <v>356</v>
-      </c>
-      <c r="I93" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="94" spans="3:14" x14ac:dyDescent="0.3">
@@ -4725,23 +4725,23 @@
         <v>292</v>
       </c>
       <c r="I123" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="124" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="F124" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G124" s="1">
         <v>66</v>
       </c>
       <c r="H124" t="s">
+        <v>441</v>
+      </c>
+      <c r="I124" s="3" t="s">
         <v>442</v>
-      </c>
-      <c r="I124" s="3" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="125" spans="3:17" x14ac:dyDescent="0.3">
@@ -4757,17 +4757,17 @@
         <v>293</v>
       </c>
       <c r="I125" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Q125" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="126" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="F126" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G126" s="1">
         <v>74</v>
@@ -4777,7 +4777,7 @@
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="F127" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G127" s="1">
         <v>140</v>
@@ -4786,7 +4786,7 @@
         <v>294</v>
       </c>
       <c r="I127" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="128" spans="3:17" x14ac:dyDescent="0.3">
@@ -4796,7 +4796,7 @@
         <v>295</v>
       </c>
       <c r="I128" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="129" spans="3:18" x14ac:dyDescent="0.3">
@@ -4807,10 +4807,10 @@
         <v>296</v>
       </c>
       <c r="I129" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="R129" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="130" spans="3:18" x14ac:dyDescent="0.3">
@@ -4869,10 +4869,10 @@
       <c r="D136" s="1"/>
       <c r="G136" s="1"/>
       <c r="H136" t="s">
+        <v>424</v>
+      </c>
+      <c r="I136" t="s">
         <v>425</v>
-      </c>
-      <c r="I136" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="137" spans="3:18" x14ac:dyDescent="0.3">
@@ -4880,106 +4880,106 @@
       <c r="D137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" t="s">
+        <v>426</v>
+      </c>
+      <c r="I137" t="s">
         <v>427</v>
-      </c>
-      <c r="I137" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="138" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="F138" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G138" s="1">
         <v>165</v>
       </c>
       <c r="H138" t="s">
+        <v>444</v>
+      </c>
+      <c r="I138" t="s">
         <v>445</v>
-      </c>
-      <c r="I138" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="139" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="F139" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G139" s="1">
         <v>173</v>
       </c>
       <c r="H139" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I139" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="140" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="F140" s="10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G140" s="1">
         <v>181</v>
       </c>
       <c r="H140" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I140" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="141" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="F141" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G141" s="1">
         <v>210</v>
       </c>
       <c r="H141" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I141" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="142" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="F142" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G142" s="1">
         <v>280</v>
       </c>
       <c r="H142" t="s">
+        <v>458</v>
+      </c>
+      <c r="I142" t="s">
         <v>459</v>
-      </c>
-      <c r="I142" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="143" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="F143" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G143" s="1">
         <v>500</v>
       </c>
       <c r="H143" t="s">
+        <v>461</v>
+      </c>
+      <c r="I143" t="s">
         <v>462</v>
-      </c>
-      <c r="I143" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="144" spans="3:18" x14ac:dyDescent="0.3">
@@ -5165,7 +5165,7 @@
         <v>241</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
@@ -5183,7 +5183,7 @@
         <v>241</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J157" s="3"/>
       <c r="K157" s="3"/>
@@ -5204,10 +5204,10 @@
         <v>800</v>
       </c>
       <c r="H158" t="s">
+        <v>438</v>
+      </c>
+      <c r="I158" s="3" t="s">
         <v>439</v>
-      </c>
-      <c r="I158" s="3" t="s">
-        <v>440</v>
       </c>
       <c r="K158" s="3"/>
       <c r="L158" s="3"/>
@@ -5222,10 +5222,10 @@
       <c r="D159" s="1"/>
       <c r="G159" s="1"/>
       <c r="H159" t="s">
+        <v>436</v>
+      </c>
+      <c r="I159" s="3" t="s">
         <v>437</v>
-      </c>
-      <c r="I159" s="3" t="s">
-        <v>438</v>
       </c>
       <c r="J159" s="3"/>
       <c r="K159" s="3"/>
@@ -5246,10 +5246,10 @@
         <v>1600</v>
       </c>
       <c r="H160" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I160" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J160" s="3"/>
       <c r="K160" s="3"/>
@@ -5633,16 +5633,16 @@
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
       <c r="F179" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G179" s="1">
         <v>170</v>
       </c>
       <c r="H179" t="s">
+        <v>340</v>
+      </c>
+      <c r="I179" t="s">
         <v>341</v>
-      </c>
-      <c r="I179" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="180" spans="3:17" x14ac:dyDescent="0.3">
@@ -5653,13 +5653,13 @@
         <v>337</v>
       </c>
       <c r="G180" s="1">
-        <v>95</v>
+        <v>95000</v>
       </c>
       <c r="H180" t="s">
+        <v>467</v>
+      </c>
+      <c r="I180" t="s">
         <v>338</v>
-      </c>
-      <c r="I180" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="181" spans="3:17" x14ac:dyDescent="0.3">
@@ -5667,29 +5667,29 @@
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
       <c r="F181" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G181" s="1">
         <v>160000</v>
       </c>
       <c r="H181" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="182" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C182" s="8"/>
       <c r="D182" s="1"/>
       <c r="E182" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F182" t="s">
         <v>385</v>
       </c>
-      <c r="F182" t="s">
+      <c r="H182" t="s">
         <v>386</v>
       </c>
-      <c r="H182" t="s">
+      <c r="I182" t="s">
         <v>387</v>
-      </c>
-      <c r="I182" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="183" spans="3:17" x14ac:dyDescent="0.3">
@@ -5700,10 +5700,10 @@
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
       <c r="H184" t="s">
+        <v>342</v>
+      </c>
+      <c r="I184" t="s">
         <v>343</v>
-      </c>
-      <c r="I184" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="185" spans="3:17" x14ac:dyDescent="0.3">

</xml_diff>